<commit_message>
resources and introductory update
</commit_message>
<xml_diff>
--- a/resources/creole_data/Konpe.xlsx
+++ b/resources/creole_data/Konpe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\GitHub\llord1.github.io\resources\creole_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93553163-FE84-4181-9E8C-450689D54D2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310FB267-B24C-4C75-A636-B7A636B8894B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3BE31084-C3D6-4C3E-B9D7-3C3342FDA15C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
   <si>
     <t>I alé, i manché on pikwa, èk i mouté anlè mòso kayé, ay fouyé twou yanm la.</t>
   </si>
@@ -42,27 +42,12 @@
     <t>Creole</t>
   </si>
   <si>
-    <t>Konpé Lapen Mandé on Favè</t>
-  </si>
-  <si>
-    <t>Konpé Lapen Asks a Favor</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
-    <t>Té ni Konpé Lapen.</t>
-  </si>
-  <si>
-    <t>Konpé Lapen di kon ha i kay mandé Bondyé on gwas, pou tout moun ki palé moun mal pou yo mo.</t>
-  </si>
-  <si>
     <t>This is the story of Konpè Lapen.</t>
   </si>
   <si>
-    <t>Konpé Lapen asked God for a favor, that all those who bad talk people will die.</t>
-  </si>
-  <si>
     <t>He went and put a handle on a pickaxe, and he climbed up on a rock to dig yams there.</t>
   </si>
   <si>
@@ -90,9 +75,6 @@
     <t>Konpè Lapen took Konpè Kochon salted him, and he ate him.</t>
   </si>
   <si>
-    <t>He saw Konpé Kabwit passing.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Konpè Kabwit di, </t>
   </si>
   <si>
@@ -123,15 +105,9 @@
     <t>“E, Makoumè Pentad, vini, vini, vini.'</t>
   </si>
   <si>
-    <t xml:space="preserve">I di, "Non, mwen pa sa. M'a ni tan pou mwen vini. </t>
-  </si>
-  <si>
     <t>Mwen ka désann an vil vitman ay strétenn pou mwen ay lonmen an fiyèl.”</t>
   </si>
   <si>
-    <t xml:space="preserve">She said, "No, I can't. I don't have time. </t>
-  </si>
-  <si>
     <t>I have to go to town quickly to have my hair straightened to christen a godchild."</t>
   </si>
   <si>
@@ -177,9 +153,6 @@
     <t>He saw Konpè Mouton passing.</t>
   </si>
   <si>
-    <t>He said, "Konpè Mouton, where did you meet Makoumè Pentad?!"</t>
-  </si>
-  <si>
     <t xml:space="preserve">He said, "I met her down there. </t>
   </si>
   <si>
@@ -195,9 +168,6 @@
     <t>Bondyé, sé pa mal ng'a palé Makoumè Pentad, on!”</t>
   </si>
   <si>
-    <t>I wété la. I wè Konpè Mouton ka pasé.</t>
-  </si>
-  <si>
     <t>Konpè Mouton, koté ou jwenn Makoumè Pentad?"</t>
   </si>
   <si>
@@ -252,24 +222,15 @@
     <t>Kwik.....Kwak!</t>
   </si>
   <si>
-    <t>Sé Konpè Lapen menm ki tè mandé Bondyé gwas-la, èk sé li menm ki mò!</t>
-  </si>
-  <si>
     <t>Konpè Lapen fell to the ground.</t>
   </si>
   <si>
-    <t>Bleketek, he died!</t>
-  </si>
-  <si>
     <t>Konpè Mouton took him, salted him, and ate him.</t>
   </si>
   <si>
     <t>It was Konpè Lapen himself who asked God for the favor, and it was he himself who died!</t>
   </si>
   <si>
-    <t>The end</t>
-  </si>
-  <si>
     <t>Konpè Kochon di,</t>
   </si>
   <si>
@@ -291,9 +252,6 @@
     <t>"Sa ou ka fè la, Konpè?"</t>
   </si>
   <si>
-    <t xml:space="preserve">Konpè  Kabwit mandé'y, </t>
-  </si>
-  <si>
     <t>Konpè Kabwit asked him,</t>
   </si>
   <si>
@@ -349,6 +307,57 @@
   </si>
   <si>
     <t>"Konpè Lapen, what are you doing there?"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I wété la. </t>
+  </si>
+  <si>
+    <t>I wè Konpè Mouton ka pasé.</t>
+  </si>
+  <si>
+    <t>"Konpè Mouton, where did you meet Makoumè Pentad?"</t>
+  </si>
+  <si>
+    <t>She said,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M'a ni tan pou mwen vini. </t>
+  </si>
+  <si>
+    <t>"Non, mwen pa sa.</t>
+  </si>
+  <si>
+    <t>"No, I can't.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I don't have time. </t>
+  </si>
+  <si>
+    <t>Konpè Lapen Mandé on Favè</t>
+  </si>
+  <si>
+    <t>Konpè Lapen Asks a Favor</t>
+  </si>
+  <si>
+    <t>Té ni Konpè Lapen.</t>
+  </si>
+  <si>
+    <t>Konpè Lapen asked God for a favor, that all those who bad talk people will die.</t>
+  </si>
+  <si>
+    <t>He saw Konpè Kabwit passing.</t>
+  </si>
+  <si>
+    <t>Konpè Lapen di kon ha i kay Mandé Bondyé on gwas, pou tout moun ki palé moun mal pou yo mo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Konpè  Kabwit Mandé'y, </t>
+  </si>
+  <si>
+    <t>Sé Konpè Lapen menm ki tè Mandé Bondyé gwas-la, èk sé li menm ki mò!</t>
+  </si>
+  <si>
+    <t>and bleketek, he died!</t>
   </si>
 </sst>
 </file>
@@ -703,16 +712,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2250AD31-A54B-4837-9D34-EA5079523B29}">
-  <dimension ref="A1:B108"/>
+  <dimension ref="A1:B114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" customWidth="1"/>
-    <col min="2" max="2" width="38.5546875" customWidth="1"/>
+    <col min="1" max="1" width="82" customWidth="1"/>
+    <col min="2" max="2" width="74.109375" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
@@ -721,31 +730,31 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -753,151 +762,151 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -905,258 +914,279 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B54" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B60" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" t="s">
         <v>28</v>
-      </c>
-      <c r="B62" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="B64" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="B66" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="B68" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B70" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B72" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>52</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>31</v>
       </c>
       <c r="B74" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="B76" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="B78" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="B80" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="B82" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
+        <v>32</v>
+      </c>
+      <c r="B84" t="s">
         <v>42</v>
-      </c>
-      <c r="B84" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B86" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="B88" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B90" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B92" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B94" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>47</v>
+      </c>
+      <c r="B96" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="B98" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B100" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>13</v>
-      </c>
-      <c r="B102" t="s">
-        <v>74</v>
+      <c r="A102" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B104" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B106" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="B108" t="s">
-        <v>77</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>60</v>
+      </c>
+      <c r="B110" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>106</v>
+      </c>
+      <c r="B112" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resources and introductory updates
</commit_message>
<xml_diff>
--- a/resources/creole_data/Konpe.xlsx
+++ b/resources/creole_data/Konpe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\GitHub\llord1.github.io\resources\creole_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93553163-FE84-4181-9E8C-450689D54D2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310FB267-B24C-4C75-A636-B7A636B8894B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3BE31084-C3D6-4C3E-B9D7-3C3342FDA15C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
   <si>
     <t>I alé, i manché on pikwa, èk i mouté anlè mòso kayé, ay fouyé twou yanm la.</t>
   </si>
@@ -42,27 +42,12 @@
     <t>Creole</t>
   </si>
   <si>
-    <t>Konpé Lapen Mandé on Favè</t>
-  </si>
-  <si>
-    <t>Konpé Lapen Asks a Favor</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
-    <t>Té ni Konpé Lapen.</t>
-  </si>
-  <si>
-    <t>Konpé Lapen di kon ha i kay mandé Bondyé on gwas, pou tout moun ki palé moun mal pou yo mo.</t>
-  </si>
-  <si>
     <t>This is the story of Konpè Lapen.</t>
   </si>
   <si>
-    <t>Konpé Lapen asked God for a favor, that all those who bad talk people will die.</t>
-  </si>
-  <si>
     <t>He went and put a handle on a pickaxe, and he climbed up on a rock to dig yams there.</t>
   </si>
   <si>
@@ -90,9 +75,6 @@
     <t>Konpè Lapen took Konpè Kochon salted him, and he ate him.</t>
   </si>
   <si>
-    <t>He saw Konpé Kabwit passing.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Konpè Kabwit di, </t>
   </si>
   <si>
@@ -123,15 +105,9 @@
     <t>“E, Makoumè Pentad, vini, vini, vini.'</t>
   </si>
   <si>
-    <t xml:space="preserve">I di, "Non, mwen pa sa. M'a ni tan pou mwen vini. </t>
-  </si>
-  <si>
     <t>Mwen ka désann an vil vitman ay strétenn pou mwen ay lonmen an fiyèl.”</t>
   </si>
   <si>
-    <t xml:space="preserve">She said, "No, I can't. I don't have time. </t>
-  </si>
-  <si>
     <t>I have to go to town quickly to have my hair straightened to christen a godchild."</t>
   </si>
   <si>
@@ -177,9 +153,6 @@
     <t>He saw Konpè Mouton passing.</t>
   </si>
   <si>
-    <t>He said, "Konpè Mouton, where did you meet Makoumè Pentad?!"</t>
-  </si>
-  <si>
     <t xml:space="preserve">He said, "I met her down there. </t>
   </si>
   <si>
@@ -195,9 +168,6 @@
     <t>Bondyé, sé pa mal ng'a palé Makoumè Pentad, on!”</t>
   </si>
   <si>
-    <t>I wété la. I wè Konpè Mouton ka pasé.</t>
-  </si>
-  <si>
     <t>Konpè Mouton, koté ou jwenn Makoumè Pentad?"</t>
   </si>
   <si>
@@ -252,24 +222,15 @@
     <t>Kwik.....Kwak!</t>
   </si>
   <si>
-    <t>Sé Konpè Lapen menm ki tè mandé Bondyé gwas-la, èk sé li menm ki mò!</t>
-  </si>
-  <si>
     <t>Konpè Lapen fell to the ground.</t>
   </si>
   <si>
-    <t>Bleketek, he died!</t>
-  </si>
-  <si>
     <t>Konpè Mouton took him, salted him, and ate him.</t>
   </si>
   <si>
     <t>It was Konpè Lapen himself who asked God for the favor, and it was he himself who died!</t>
   </si>
   <si>
-    <t>The end</t>
-  </si>
-  <si>
     <t>Konpè Kochon di,</t>
   </si>
   <si>
@@ -291,9 +252,6 @@
     <t>"Sa ou ka fè la, Konpè?"</t>
   </si>
   <si>
-    <t xml:space="preserve">Konpè  Kabwit mandé'y, </t>
-  </si>
-  <si>
     <t>Konpè Kabwit asked him,</t>
   </si>
   <si>
@@ -349,6 +307,57 @@
   </si>
   <si>
     <t>"Konpè Lapen, what are you doing there?"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I wété la. </t>
+  </si>
+  <si>
+    <t>I wè Konpè Mouton ka pasé.</t>
+  </si>
+  <si>
+    <t>"Konpè Mouton, where did you meet Makoumè Pentad?"</t>
+  </si>
+  <si>
+    <t>She said,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M'a ni tan pou mwen vini. </t>
+  </si>
+  <si>
+    <t>"Non, mwen pa sa.</t>
+  </si>
+  <si>
+    <t>"No, I can't.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I don't have time. </t>
+  </si>
+  <si>
+    <t>Konpè Lapen Mandé on Favè</t>
+  </si>
+  <si>
+    <t>Konpè Lapen Asks a Favor</t>
+  </si>
+  <si>
+    <t>Té ni Konpè Lapen.</t>
+  </si>
+  <si>
+    <t>Konpè Lapen asked God for a favor, that all those who bad talk people will die.</t>
+  </si>
+  <si>
+    <t>He saw Konpè Kabwit passing.</t>
+  </si>
+  <si>
+    <t>Konpè Lapen di kon ha i kay Mandé Bondyé on gwas, pou tout moun ki palé moun mal pou yo mo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Konpè  Kabwit Mandé'y, </t>
+  </si>
+  <si>
+    <t>Sé Konpè Lapen menm ki tè Mandé Bondyé gwas-la, èk sé li menm ki mò!</t>
+  </si>
+  <si>
+    <t>and bleketek, he died!</t>
   </si>
 </sst>
 </file>
@@ -703,16 +712,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2250AD31-A54B-4837-9D34-EA5079523B29}">
-  <dimension ref="A1:B108"/>
+  <dimension ref="A1:B114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" customWidth="1"/>
-    <col min="2" max="2" width="38.5546875" customWidth="1"/>
+    <col min="1" max="1" width="82" customWidth="1"/>
+    <col min="2" max="2" width="74.109375" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
@@ -721,31 +730,31 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -753,151 +762,151 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -905,258 +914,279 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B54" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B60" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" t="s">
         <v>28</v>
-      </c>
-      <c r="B62" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="B64" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="B66" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="B68" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B70" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B72" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>52</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>31</v>
       </c>
       <c r="B74" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="B76" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="B78" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="B80" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="B82" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
+        <v>32</v>
+      </c>
+      <c r="B84" t="s">
         <v>42</v>
-      </c>
-      <c r="B84" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B86" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="B88" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B90" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B92" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B94" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>47</v>
+      </c>
+      <c r="B96" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="B98" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B100" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>13</v>
-      </c>
-      <c r="B102" t="s">
-        <v>74</v>
+      <c r="A102" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B104" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B106" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="B108" t="s">
-        <v>77</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>60</v>
+      </c>
+      <c r="B110" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>106</v>
+      </c>
+      <c r="B112" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>